<commit_message>
Added pictures; Changed view option for app
</commit_message>
<xml_diff>
--- a/Заявка.xlsx
+++ b/Заявка.xlsx
@@ -462,13 +462,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C2" t="n">
         <v>1</v>
       </c>
       <c r="D2" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3">
@@ -494,13 +494,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C4" t="n">
         <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5">

</xml_diff>